<commit_message>
created documentation branch with ERD and initial risk assessment
</commit_message>
<xml_diff>
--- a/Initial Risk Assessment.xlsx
+++ b/Initial Risk Assessment.xlsx
@@ -178,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +188,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -253,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +546,7 @@
   <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,7 +563,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>